<commit_message>
let's bring this puppy up to date
</commit_message>
<xml_diff>
--- a/BMRtest.xlsx
+++ b/BMRtest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="26680" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="26680" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="385">
   <si>
     <t>Species</t>
   </si>
@@ -1178,6 +1178,12 @@
   </si>
   <si>
     <t>blossom bat</t>
+  </si>
+  <si>
+    <t>Langman</t>
+  </si>
+  <si>
+    <t>Elephant</t>
   </si>
 </sst>
 </file>
@@ -1552,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73:J83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5711,6 +5717,28 @@
         <v>46</v>
       </c>
       <c r="L127" s="1"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B128" s="3"/>
+      <c r="D128" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F128" s="1">
+        <v>1542</v>
+      </c>
+      <c r="G128">
+        <f>5550*24</f>
+        <v>133200</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I128" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>